<commit_message>
Cambiando Nombre a Columna
</commit_message>
<xml_diff>
--- a/Calendar_Datafest.xlsx
+++ b/Calendar_Datafest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Datafest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB83FA1-12EB-49F9-83F6-B317F042B473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DB41CA-F12B-4716-9501-8FFF271F9060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F16FAED0-20E3-4A3A-81E9-0E87612026F7}"/>
+    <workbookView xWindow="16215" yWindow="0" windowWidth="9855" windowHeight="10530" xr2:uid="{F16FAED0-20E3-4A3A-81E9-0E87612026F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>HolidayType</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>HoliDay</t>
+  </si>
+  <si>
+    <t>SpecialDates</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:G167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,16 +541,16 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4" t="str">
         <f>_xlfn.CONCAT(A2,"-",C2,"-",D2)</f>
@@ -589,7 +589,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F66" si="0">_xlfn.CONCAT(A3,"-",C3,"-",D3)</f>
@@ -610,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -652,7 +652,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -673,7 +673,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -715,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -736,7 +736,7 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -757,7 +757,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -778,7 +778,7 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -799,7 +799,7 @@
         <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -820,7 +820,7 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -841,7 +841,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -862,7 +862,7 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -904,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -925,7 +925,7 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -946,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -967,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -988,7 +988,7 @@
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -1009,7 +1009,7 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -1030,7 +1030,7 @@
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -1072,7 +1072,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -1093,7 +1093,7 @@
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -1114,7 +1114,7 @@
         <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -1135,7 +1135,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -1156,7 +1156,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -1177,7 +1177,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -1198,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -1219,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -1240,7 +1240,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -1261,7 +1261,7 @@
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
@@ -1282,7 +1282,7 @@
         <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -1303,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -1324,7 +1324,7 @@
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -1345,7 +1345,7 @@
         <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
@@ -1366,7 +1366,7 @@
         <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
@@ -1387,7 +1387,7 @@
         <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -1408,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -1429,7 +1429,7 @@
         <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -1450,7 +1450,7 @@
         <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
@@ -1471,7 +1471,7 @@
         <v>29</v>
       </c>
       <c r="E45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -1492,7 +1492,7 @@
         <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -1513,7 +1513,7 @@
         <v>28</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
@@ -1534,7 +1534,7 @@
         <v>29</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
@@ -1555,7 +1555,7 @@
         <v>30</v>
       </c>
       <c r="E49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
@@ -1576,7 +1576,7 @@
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
@@ -1618,7 +1618,7 @@
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
@@ -1639,7 +1639,7 @@
         <v>25</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
@@ -1681,7 +1681,7 @@
         <v>14</v>
       </c>
       <c r="E55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
@@ -1702,7 +1702,7 @@
         <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
@@ -1723,7 +1723,7 @@
         <v>30</v>
       </c>
       <c r="E57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
@@ -1744,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
@@ -1765,7 +1765,7 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
@@ -1786,7 +1786,7 @@
         <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
@@ -1807,7 +1807,7 @@
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
@@ -1828,7 +1828,7 @@
         <v>24</v>
       </c>
       <c r="E62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
@@ -1849,7 +1849,7 @@
         <v>29</v>
       </c>
       <c r="E63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
@@ -1870,7 +1870,7 @@
         <v>28</v>
       </c>
       <c r="E64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
@@ -1891,7 +1891,7 @@
         <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
@@ -1912,7 +1912,7 @@
         <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
@@ -1933,7 +1933,7 @@
         <v>8</v>
       </c>
       <c r="E67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" ref="F67:F130" si="1">_xlfn.CONCAT(A67,"-",C67,"-",D67)</f>
@@ -1954,7 +1954,7 @@
         <v>14</v>
       </c>
       <c r="E68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
@@ -1975,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
@@ -1996,7 +1996,7 @@
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
@@ -2017,7 +2017,7 @@
         <v>25</v>
       </c>
       <c r="E71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
@@ -2038,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
@@ -2059,7 +2059,7 @@
         <v>14</v>
       </c>
       <c r="E73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
@@ -2080,7 +2080,7 @@
         <v>18</v>
       </c>
       <c r="E74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
@@ -2101,7 +2101,7 @@
         <v>19</v>
       </c>
       <c r="E75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
@@ -2122,7 +2122,7 @@
         <v>21</v>
       </c>
       <c r="E76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
@@ -2143,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
@@ -2164,7 +2164,7 @@
         <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
@@ -2185,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
@@ -2206,7 +2206,7 @@
         <v>29</v>
       </c>
       <c r="E80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
@@ -2227,7 +2227,7 @@
         <v>26</v>
       </c>
       <c r="E81" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
@@ -2248,7 +2248,7 @@
         <v>27</v>
       </c>
       <c r="E82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
@@ -2269,7 +2269,7 @@
         <v>28</v>
       </c>
       <c r="E83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
@@ -2290,7 +2290,7 @@
         <v>29</v>
       </c>
       <c r="E84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
@@ -2311,7 +2311,7 @@
         <v>29</v>
       </c>
       <c r="E85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
@@ -2332,7 +2332,7 @@
         <v>30</v>
       </c>
       <c r="E86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
@@ -2353,7 +2353,7 @@
         <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
@@ -2374,7 +2374,7 @@
         <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
@@ -2395,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
@@ -2416,7 +2416,7 @@
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
@@ -2437,7 +2437,7 @@
         <v>25</v>
       </c>
       <c r="E91" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
@@ -2458,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
@@ -2479,7 +2479,7 @@
         <v>14</v>
       </c>
       <c r="E93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
@@ -2500,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
@@ -2521,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="E95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
@@ -2542,7 +2542,7 @@
         <v>4</v>
       </c>
       <c r="E96" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
@@ -2563,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
@@ -2584,7 +2584,7 @@
         <v>9</v>
       </c>
       <c r="E98" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
@@ -2605,7 +2605,7 @@
         <v>20</v>
       </c>
       <c r="E99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
@@ -2626,7 +2626,7 @@
         <v>29</v>
       </c>
       <c r="E100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
@@ -2647,7 +2647,7 @@
         <v>28</v>
       </c>
       <c r="E101" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
@@ -2668,7 +2668,7 @@
         <v>29</v>
       </c>
       <c r="E102" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
@@ -2689,7 +2689,7 @@
         <v>30</v>
       </c>
       <c r="E103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
@@ -2710,7 +2710,7 @@
         <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
@@ -2731,7 +2731,7 @@
         <v>10</v>
       </c>
       <c r="E105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
@@ -2752,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
@@ -2773,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="E107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
@@ -2794,7 +2794,7 @@
         <v>25</v>
       </c>
       <c r="E108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
@@ -2815,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
@@ -2836,7 +2836,7 @@
         <v>14</v>
       </c>
       <c r="E110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
@@ -2857,7 +2857,7 @@
         <v>14</v>
       </c>
       <c r="E111" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
@@ -2878,7 +2878,7 @@
         <v>15</v>
       </c>
       <c r="E112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
@@ -2899,7 +2899,7 @@
         <v>17</v>
       </c>
       <c r="E113" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
@@ -2920,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
@@ -2941,7 +2941,7 @@
         <v>8</v>
       </c>
       <c r="E115" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
@@ -2962,7 +2962,7 @@
         <v>19</v>
       </c>
       <c r="E116" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
@@ -2983,7 +2983,7 @@
         <v>29</v>
       </c>
       <c r="E117" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
@@ -3004,7 +3004,7 @@
         <v>28</v>
       </c>
       <c r="E118" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="1"/>
@@ -3025,7 +3025,7 @@
         <v>29</v>
       </c>
       <c r="E119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="1"/>
@@ -3046,7 +3046,7 @@
         <v>6</v>
       </c>
       <c r="E120" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="1"/>
@@ -3067,7 +3067,7 @@
         <v>30</v>
       </c>
       <c r="E121" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="1"/>
@@ -3088,7 +3088,7 @@
         <v>8</v>
       </c>
       <c r="E122" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
@@ -3109,7 +3109,7 @@
         <v>9</v>
       </c>
       <c r="E123" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
@@ -3130,7 +3130,7 @@
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
@@ -3151,7 +3151,7 @@
         <v>8</v>
       </c>
       <c r="E125" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="1"/>
@@ -3172,7 +3172,7 @@
         <v>9</v>
       </c>
       <c r="E126" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="1"/>
@@ -3193,7 +3193,7 @@
         <v>25</v>
       </c>
       <c r="E127" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="1"/>
@@ -3214,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="E128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
@@ -3235,7 +3235,7 @@
         <v>14</v>
       </c>
       <c r="E129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="1"/>
@@ -3256,7 +3256,7 @@
         <v>6</v>
       </c>
       <c r="E130" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F130" t="str">
         <f t="shared" si="1"/>
@@ -3277,7 +3277,7 @@
         <v>7</v>
       </c>
       <c r="E131" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F131" t="str">
         <f t="shared" ref="F131:F167" si="2">_xlfn.CONCAT(A131,"-",C131,"-",D131)</f>
@@ -3298,7 +3298,7 @@
         <v>9</v>
       </c>
       <c r="E132" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F132" t="str">
         <f t="shared" si="2"/>
@@ -3319,7 +3319,7 @@
         <v>1</v>
       </c>
       <c r="E133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="2"/>
@@ -3340,7 +3340,7 @@
         <v>14</v>
       </c>
       <c r="E134" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F134" t="str">
         <f t="shared" si="2"/>
@@ -3361,7 +3361,7 @@
         <v>18</v>
       </c>
       <c r="E135" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="2"/>
@@ -3382,7 +3382,7 @@
         <v>29</v>
       </c>
       <c r="E136" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="2"/>
@@ -3403,7 +3403,7 @@
         <v>23</v>
       </c>
       <c r="E137" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="2"/>
@@ -3424,7 +3424,7 @@
         <v>28</v>
       </c>
       <c r="E138" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="2"/>
@@ -3445,7 +3445,7 @@
         <v>29</v>
       </c>
       <c r="E139" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F139" t="str">
         <f t="shared" si="2"/>
@@ -3466,7 +3466,7 @@
         <v>6</v>
       </c>
       <c r="E140" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F140" t="str">
         <f t="shared" si="2"/>
@@ -3487,7 +3487,7 @@
         <v>30</v>
       </c>
       <c r="E141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="2"/>
@@ -3508,7 +3508,7 @@
         <v>8</v>
       </c>
       <c r="E142" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="2"/>
@@ -3529,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="2"/>
@@ -3550,7 +3550,7 @@
         <v>8</v>
       </c>
       <c r="E144" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="2"/>
@@ -3571,7 +3571,7 @@
         <v>9</v>
       </c>
       <c r="E145" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="2"/>
@@ -3592,7 +3592,7 @@
         <v>25</v>
       </c>
       <c r="E146" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="2"/>
@@ -3613,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="E147" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F147" t="str">
         <f t="shared" si="2"/>
@@ -3634,7 +3634,7 @@
         <v>14</v>
       </c>
       <c r="E148" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F148" t="str">
         <f t="shared" si="2"/>
@@ -3655,7 +3655,7 @@
         <v>28</v>
       </c>
       <c r="E149" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F149" t="str">
         <f t="shared" si="2"/>
@@ -3676,7 +3676,7 @@
         <v>29</v>
       </c>
       <c r="E150" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F150" t="str">
         <f t="shared" si="2"/>
@@ -3697,7 +3697,7 @@
         <v>31</v>
       </c>
       <c r="E151" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F151" t="str">
         <f t="shared" si="2"/>
@@ -3718,7 +3718,7 @@
         <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F152" t="str">
         <f t="shared" si="2"/>
@@ -3739,7 +3739,7 @@
         <v>12</v>
       </c>
       <c r="E153" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F153" t="str">
         <f t="shared" si="2"/>
@@ -3760,7 +3760,7 @@
         <v>7</v>
       </c>
       <c r="E154" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F154" t="str">
         <f t="shared" si="2"/>
@@ -3781,7 +3781,7 @@
         <v>16</v>
       </c>
       <c r="E155" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F155" t="str">
         <f t="shared" si="2"/>
@@ -3802,7 +3802,7 @@
         <v>29</v>
       </c>
       <c r="E156" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F156" t="str">
         <f t="shared" si="2"/>
@@ -3823,7 +3823,7 @@
         <v>23</v>
       </c>
       <c r="E157" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="2"/>
@@ -3844,7 +3844,7 @@
         <v>28</v>
       </c>
       <c r="E158" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="2"/>
@@ -3865,7 +3865,7 @@
         <v>29</v>
       </c>
       <c r="E159" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="2"/>
@@ -3886,7 +3886,7 @@
         <v>6</v>
       </c>
       <c r="E160" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F160" t="str">
         <f t="shared" si="2"/>
@@ -3907,7 +3907,7 @@
         <v>30</v>
       </c>
       <c r="E161" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F161" t="str">
         <f t="shared" si="2"/>
@@ -3928,7 +3928,7 @@
         <v>8</v>
       </c>
       <c r="E162" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F162" t="str">
         <f t="shared" si="2"/>
@@ -3949,7 +3949,7 @@
         <v>13</v>
       </c>
       <c r="E163" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F163" t="str">
         <f t="shared" si="2"/>
@@ -3970,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="E164" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="2"/>
@@ -3991,7 +3991,7 @@
         <v>8</v>
       </c>
       <c r="E165" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F165" t="str">
         <f t="shared" si="2"/>
@@ -4012,7 +4012,7 @@
         <v>9</v>
       </c>
       <c r="E166" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F166" t="str">
         <f t="shared" si="2"/>
@@ -4033,7 +4033,7 @@
         <v>25</v>
       </c>
       <c r="E167" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Cambiando Nombre a Columna ImportantDates
</commit_message>
<xml_diff>
--- a/Calendar_Datafest.xlsx
+++ b/Calendar_Datafest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Datafest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DB41CA-F12B-4716-9501-8FFF271F9060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE0259D-7352-49A9-9129-675A8CD4FB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16215" yWindow="0" windowWidth="9855" windowHeight="10530" xr2:uid="{F16FAED0-20E3-4A3A-81E9-0E87612026F7}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>HoliDay</t>
   </si>
   <si>
-    <t>SpecialDates</t>
+    <t>ImportantDates</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:G167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cambiando Nombre a Columna ImportantDate
</commit_message>
<xml_diff>
--- a/Calendar_Datafest.xlsx
+++ b/Calendar_Datafest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Datafest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE0259D-7352-49A9-9129-675A8CD4FB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC8DC81-78FA-4DCE-B041-FAC57B234110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16215" yWindow="0" windowWidth="9855" windowHeight="10530" xr2:uid="{F16FAED0-20E3-4A3A-81E9-0E87612026F7}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>HoliDay</t>
   </si>
   <si>
-    <t>ImportantDates</t>
+    <t>ImportantDate</t>
   </si>
 </sst>
 </file>
@@ -524,12 +524,12 @@
   <dimension ref="A1:G167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>